<commit_message>
Arreglo descarga de XMLs en ZIP
</commit_message>
<xml_diff>
--- a/nominas/BIO870307QD0/Reporte de Nomina  2023-01-20.xlsx
+++ b/nominas/BIO870307QD0/Reporte de Nomina  2023-01-20.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="965">
   <si>
     <t>Emite: Oscar Farias Ayala</t>
   </si>
@@ -2307,6 +2307,609 @@
   </si>
   <si>
     <t>S:::Subsidio Causado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>$ 513.44</t>
+  </si>
+  <si>
+    <t>$ 7,188.16</t>
+  </si>
+  <si>
+    <t>$ 503.18</t>
+  </si>
+  <si>
+    <t>$ 384.88</t>
+  </si>
+  <si>
+    <t>$ 565.84</t>
+  </si>
+  <si>
+    <t>$ 342.52</t>
+  </si>
+  <si>
+    <t>$ 671.74</t>
+  </si>
+  <si>
+    <t>$ 9,404.36</t>
+  </si>
+  <si>
+    <t>$ 658.30</t>
+  </si>
+  <si>
+    <t>$ 859.38</t>
+  </si>
+  <si>
+    <t>$ 464.55</t>
+  </si>
+  <si>
+    <t>$ 1,914.48</t>
+  </si>
+  <si>
+    <t>$ 26,802.72</t>
+  </si>
+  <si>
+    <t>$ 1,876.20</t>
+  </si>
+  <si>
+    <t>$ 4,498.42</t>
+  </si>
+  <si>
+    <t>$ 1,261.26</t>
+  </si>
+  <si>
+    <t>$ 2,085.04</t>
+  </si>
+  <si>
+    <t>$ 29,190.56</t>
+  </si>
+  <si>
+    <t>$ 2,043.34</t>
+  </si>
+  <si>
+    <t>$ 5,043.18</t>
+  </si>
+  <si>
+    <t>$ 1,355.05</t>
+  </si>
+  <si>
+    <t>$ 7,866.10</t>
+  </si>
+  <si>
+    <t>$ 657.90</t>
+  </si>
+  <si>
+    <t>$ 9,210.60</t>
+  </si>
+  <si>
+    <t>$ 644.74</t>
+  </si>
+  <si>
+    <t>$ 831.48</t>
+  </si>
+  <si>
+    <t>$ 530.38</t>
+  </si>
+  <si>
+    <t>$ 450.00</t>
+  </si>
+  <si>
+    <t>$ 893.56</t>
+  </si>
+  <si>
+    <t>$ 543.06</t>
+  </si>
+  <si>
+    <t>$ 7,602.84</t>
+  </si>
+  <si>
+    <t>$ 532.20</t>
+  </si>
+  <si>
+    <t>$ 720.78</t>
+  </si>
+  <si>
+    <t>$ 397.71</t>
+  </si>
+  <si>
+    <t>$ 1,412.00</t>
+  </si>
+  <si>
+    <t>$ 1,000.94</t>
+  </si>
+  <si>
+    <t>$ 14,013.16</t>
+  </si>
+  <si>
+    <t>$ 980.92</t>
+  </si>
+  <si>
+    <t>$ 1,799.32</t>
+  </si>
+  <si>
+    <t>$ 752.99</t>
+  </si>
+  <si>
+    <t>$ 3,461.62</t>
+  </si>
+  <si>
+    <t>$ 719.14</t>
+  </si>
+  <si>
+    <t>$ 10,067.96</t>
+  </si>
+  <si>
+    <t>$ 704.76</t>
+  </si>
+  <si>
+    <t>$ 1,215.67</t>
+  </si>
+  <si>
+    <t>$ 580.63</t>
+  </si>
+  <si>
+    <t>$ 1,300.00</t>
+  </si>
+  <si>
+    <t>$ 2,356.20</t>
+  </si>
+  <si>
+    <t>$ 32,986.80</t>
+  </si>
+  <si>
+    <t>$ 2,309.08</t>
+  </si>
+  <si>
+    <t>$ 5,936.05</t>
+  </si>
+  <si>
+    <t>$ 1,125.98</t>
+  </si>
+  <si>
+    <t>$ 6,000.00</t>
+  </si>
+  <si>
+    <t>$ 756.58</t>
+  </si>
+  <si>
+    <t>$ 10,592.12</t>
+  </si>
+  <si>
+    <t>$ 741.44</t>
+  </si>
+  <si>
+    <t>$ 1,369.09</t>
+  </si>
+  <si>
+    <t>$ 550.77</t>
+  </si>
+  <si>
+    <t>$ 960.69</t>
+  </si>
+  <si>
+    <t>$ 483.22</t>
+  </si>
+  <si>
+    <t>$ 1,895.24</t>
+  </si>
+  <si>
+    <t>$ 3,956.26</t>
+  </si>
+  <si>
+    <t>$ 55,387.64</t>
+  </si>
+  <si>
+    <t>$ 2,215.50</t>
+  </si>
+  <si>
+    <t>$ 12,210.96</t>
+  </si>
+  <si>
+    <t>$ 1,741.74</t>
+  </si>
+  <si>
+    <t>$ 6,500.00</t>
+  </si>
+  <si>
+    <t>$ 828.04</t>
+  </si>
+  <si>
+    <t>$ 11,592.56</t>
+  </si>
+  <si>
+    <t>$ 811.48</t>
+  </si>
+  <si>
+    <t>$ 1,379.18</t>
+  </si>
+  <si>
+    <t>$ 605.23</t>
+  </si>
+  <si>
+    <t>$ 70.76</t>
+  </si>
+  <si>
+    <t>$ 757.00</t>
+  </si>
+  <si>
+    <t>$ 10,598.00</t>
+  </si>
+  <si>
+    <t>$ 741.86</t>
+  </si>
+  <si>
+    <t>$ 1,050.59</t>
+  </si>
+  <si>
+    <t>$ 480.47</t>
+  </si>
+  <si>
+    <t>$ 427.64</t>
+  </si>
+  <si>
+    <t>$ 5,986.96</t>
+  </si>
+  <si>
+    <t>$ 201.62</t>
+  </si>
+  <si>
+    <t>$ 159.51</t>
+  </si>
+  <si>
+    <t>$ 233.52</t>
+  </si>
+  <si>
+    <t>$ 1,737.78</t>
+  </si>
+  <si>
+    <t>$ 24,328.92</t>
+  </si>
+  <si>
+    <t>$ 1,703.02</t>
+  </si>
+  <si>
+    <t>$ 3,943.30</t>
+  </si>
+  <si>
+    <t>$ 1,173.99</t>
+  </si>
+  <si>
+    <t>$ 7,331.31</t>
+  </si>
+  <si>
+    <t>$ 513.19</t>
+  </si>
+  <si>
+    <t>$ 365.64</t>
+  </si>
+  <si>
+    <t>$ 321.04</t>
+  </si>
+  <si>
+    <t>$ 394.94</t>
+  </si>
+  <si>
+    <t>$ 5,529.16</t>
+  </si>
+  <si>
+    <t>$ 387.04</t>
+  </si>
+  <si>
+    <t>$ 151.82</t>
+  </si>
+  <si>
+    <t>$ 242.52</t>
+  </si>
+  <si>
+    <t>$ 709.20</t>
+  </si>
+  <si>
+    <t>$ 1,051.47</t>
+  </si>
+  <si>
+    <t>$ 497.42</t>
+  </si>
+  <si>
+    <t>$ 642.28</t>
+  </si>
+  <si>
+    <t>$ 8,991.92</t>
+  </si>
+  <si>
+    <t>$ 629.44</t>
+  </si>
+  <si>
+    <t>$ 799.99</t>
+  </si>
+  <si>
+    <t>$ 398.38</t>
+  </si>
+  <si>
+    <t>$ 611.98</t>
+  </si>
+  <si>
+    <t>$ 296.41</t>
+  </si>
+  <si>
+    <t>$ 552.92</t>
+  </si>
+  <si>
+    <t>$ 7,740.88</t>
+  </si>
+  <si>
+    <t>$ 541.86</t>
+  </si>
+  <si>
+    <t>$ 855.11</t>
+  </si>
+  <si>
+    <t>$ 475.11</t>
+  </si>
+  <si>
+    <t>$ 1,559.60</t>
+  </si>
+  <si>
+    <t>$ 690.80</t>
+  </si>
+  <si>
+    <t>$ 9,671.20</t>
+  </si>
+  <si>
+    <t>$ 676.98</t>
+  </si>
+  <si>
+    <t>$ 1,423.18</t>
+  </si>
+  <si>
+    <t>$ 523.82</t>
+  </si>
+  <si>
+    <t>$ 423.62</t>
+  </si>
+  <si>
+    <t>$ 5,930.68</t>
+  </si>
+  <si>
+    <t>$ 415.14</t>
+  </si>
+  <si>
+    <t>$ 366.66</t>
+  </si>
+  <si>
+    <t>$ 506.84</t>
+  </si>
+  <si>
+    <t>$ 7,095.76</t>
+  </si>
+  <si>
+    <t>$ 496.70</t>
+  </si>
+  <si>
+    <t>$ 555.78</t>
+  </si>
+  <si>
+    <t>$ 332.19</t>
+  </si>
+  <si>
+    <t>$ 2,528.28</t>
+  </si>
+  <si>
+    <t>$ 1,407.60</t>
+  </si>
+  <si>
+    <t>$ 19,706.40</t>
+  </si>
+  <si>
+    <t>$ 1,379.44</t>
+  </si>
+  <si>
+    <t>$ 2,847.75</t>
+  </si>
+  <si>
+    <t>$ 795.37</t>
+  </si>
+  <si>
+    <t>$ 1,135.48</t>
+  </si>
+  <si>
+    <t>$ 15,896.72</t>
+  </si>
+  <si>
+    <t>$ 1,112.78</t>
+  </si>
+  <si>
+    <t>$ 2,116.22</t>
+  </si>
+  <si>
+    <t>$ 852.19</t>
+  </si>
+  <si>
+    <t>$ 1,200.00</t>
+  </si>
+  <si>
+    <t>$ 4,124.10</t>
+  </si>
+  <si>
+    <t>$ 273.41</t>
+  </si>
+  <si>
+    <t>$ 828.40</t>
+  </si>
+  <si>
+    <t>$ 11,597.60</t>
+  </si>
+  <si>
+    <t>$ 811.84</t>
+  </si>
+  <si>
+    <t>$ 1,236.81</t>
+  </si>
+  <si>
+    <t>$ 528.10</t>
+  </si>
+  <si>
+    <t>$ 2,391.04</t>
+  </si>
+  <si>
+    <t>$ 592.10</t>
+  </si>
+  <si>
+    <t>$ 8,289.40</t>
+  </si>
+  <si>
+    <t>$ 990.05</t>
+  </si>
+  <si>
+    <t>$ 222.94</t>
+  </si>
+  <si>
+    <t>$ 2,008.50</t>
+  </si>
+  <si>
+    <t>$ 28,119.00</t>
+  </si>
+  <si>
+    <t>$ 1,968.34</t>
+  </si>
+  <si>
+    <t>$ 4,793.79</t>
+  </si>
+  <si>
+    <t>$ 1,335.88</t>
+  </si>
+  <si>
+    <t>$ 218.01</t>
+  </si>
+  <si>
+    <t>$ 1,253.86</t>
+  </si>
+  <si>
+    <t>$ 556.38</t>
+  </si>
+  <si>
+    <t>$ 658.41</t>
+  </si>
+  <si>
+    <t>$ 332.08</t>
+  </si>
+  <si>
+    <t>$ 410.60</t>
+  </si>
+  <si>
+    <t>$ 3,628.09</t>
+  </si>
+  <si>
+    <t>$ 2,877.80</t>
+  </si>
+  <si>
+    <t>$ 40,289.20</t>
+  </si>
+  <si>
+    <t>$ 2,820.24</t>
+  </si>
+  <si>
+    <t>$ 7,832.11</t>
+  </si>
+  <si>
+    <t>$ 1,517.75</t>
+  </si>
+  <si>
+    <t>$ 1,400.00</t>
+  </si>
+  <si>
+    <t>$ 1,447.36</t>
+  </si>
+  <si>
+    <t>$ 20,263.04</t>
+  </si>
+  <si>
+    <t>$ 1,418.42</t>
+  </si>
+  <si>
+    <t>$ 3,048.86</t>
+  </si>
+  <si>
+    <t>$ 866.42</t>
+  </si>
+  <si>
+    <t>$ 550.00</t>
+  </si>
+  <si>
+    <t>$ 687.88</t>
+  </si>
+  <si>
+    <t>$ 9,630.32</t>
+  </si>
+  <si>
+    <t>$ 674.12</t>
+  </si>
+  <si>
+    <t>$ 966.47</t>
+  </si>
+  <si>
+    <t>$ 438.52</t>
+  </si>
+  <si>
+    <t>$ 3,338.96</t>
+  </si>
+  <si>
+    <t>$ 4,111.84</t>
+  </si>
+  <si>
+    <t>$ 57,565.76</t>
+  </si>
+  <si>
+    <t>$ 4,029.61</t>
+  </si>
+  <si>
+    <t>$ 15,864.39</t>
+  </si>
+  <si>
+    <t>$ 1,836.74</t>
+  </si>
+  <si>
+    <t>$ 1,448.16</t>
+  </si>
+  <si>
+    <t>$ 20,274.24</t>
+  </si>
+  <si>
+    <t>$ 1,419.20</t>
+  </si>
+  <si>
+    <t>$ 3,051.25</t>
+  </si>
+  <si>
+    <t>$ 1,049.81</t>
+  </si>
+  <si>
+    <t>$ 4,310.82</t>
+  </si>
+  <si>
+    <t>$ 60,351.48</t>
+  </si>
+  <si>
+    <t>$ 2,414.06</t>
+  </si>
+  <si>
+    <t>$ 13,584.64</t>
+  </si>
+  <si>
+    <t>$ 1,813.27</t>
+  </si>
+  <si>
+    <t>$ 971.47</t>
+  </si>
+  <si>
+    <t>$ 492.86</t>
+  </si>
+  <si>
+    <t>$ 839.90</t>
+  </si>
+  <si>
+    <t>$ 2,891.40</t>
   </si>
 </sst>
 </file>
@@ -2660,10 +3263,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AE144"/>
+  <dimension ref="A1:AE143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="Z143" sqref="Z143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9921,727 +10524,3438 @@
         <v>763</v>
       </c>
     </row>
+    <row r="101" spans="1:31">
+      <c r="A101" t="s">
+        <v>764</v>
+      </c>
+      <c r="B101"/>
+      <c r="C101"/>
+      <c r="D101"/>
+      <c r="E101" t="s">
+        <v>40</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q101" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="R101" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="S101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y101" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z101" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="102" spans="1:31">
-      <c r="A102"/>
-      <c r="B102"/>
-      <c r="C102"/>
-      <c r="D102"/>
-      <c r="E102">
-        <v>0</v>
+      <c r="A102" t="s">
+        <v>178</v>
+      </c>
+      <c r="B102">
+        <v>61</v>
+      </c>
+      <c r="C102" t="s">
+        <v>82</v>
+      </c>
+      <c r="D102" t="s">
+        <v>179</v>
+      </c>
+      <c r="E102" t="s">
+        <v>765</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="J102" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q102" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="R102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S102" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="T102" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="U102" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V102" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="W102" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="X102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y102" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z102" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="103" spans="1:31">
       <c r="A103" t="s">
-        <v>178</v>
+        <v>378</v>
       </c>
       <c r="B103">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="C103" t="s">
         <v>82</v>
       </c>
       <c r="D103" t="s">
-        <v>179</v>
-      </c>
-      <c r="E103">
-        <v>513.44</v>
+        <v>58</v>
+      </c>
+      <c r="E103" t="s">
+        <v>771</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q103" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="R103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S103" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="T103" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="U103" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V103" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="W103" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="X103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z103" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="104" spans="1:31">
       <c r="A104" t="s">
-        <v>378</v>
+        <v>213</v>
       </c>
       <c r="B104">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="C104" t="s">
         <v>82</v>
       </c>
       <c r="D104" t="s">
-        <v>58</v>
-      </c>
-      <c r="E104">
-        <v>671.74</v>
+        <v>214</v>
+      </c>
+      <c r="E104" t="s">
+        <v>776</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q104" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="R104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S104" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="T104" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="U104" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V104" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="W104" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="X104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z104" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="105" spans="1:31">
       <c r="A105" t="s">
-        <v>213</v>
+        <v>43</v>
       </c>
       <c r="B105">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C105" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="D105" t="s">
-        <v>214</v>
-      </c>
-      <c r="E105">
-        <v>1914.48</v>
+        <v>44</v>
+      </c>
+      <c r="E105" t="s">
+        <v>781</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q105" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="R105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S105" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="T105" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="U105" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V105" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="W105" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X105" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="Y105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z105" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="106" spans="1:31">
       <c r="A106" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="B106">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C106" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="D106" t="s">
-        <v>44</v>
-      </c>
-      <c r="E106">
-        <v>2085.04</v>
+        <v>84</v>
+      </c>
+      <c r="E106" t="s">
+        <v>787</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q106" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="R106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S106" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="T106" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="U106" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V106" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="W106" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="X106" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="Y106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z106" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="107" spans="1:31">
       <c r="A107" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="B107">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="C107" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="D107" t="s">
-        <v>84</v>
-      </c>
-      <c r="E107">
-        <v>657.9</v>
+        <v>58</v>
+      </c>
+      <c r="E107" t="s">
+        <v>794</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L107" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="M107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q107" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="R107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S107" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="T107" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="U107" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V107" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="W107" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="X107" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="Y107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z107" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="108" spans="1:31">
       <c r="A108" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="B108">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="C108" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="D108" t="s">
-        <v>58</v>
-      </c>
-      <c r="E108">
-        <v>543.06</v>
+        <v>149</v>
+      </c>
+      <c r="E108" t="s">
+        <v>800</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L108" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q108" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="R108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S108" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="T108" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="U108" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V108" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="W108" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X108" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="Y108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z108" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="109" spans="1:31">
       <c r="A109" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="B109">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C109" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D109" t="s">
-        <v>149</v>
-      </c>
-      <c r="E109">
-        <v>1000.94</v>
+        <v>173</v>
+      </c>
+      <c r="E109" t="s">
+        <v>806</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="M109" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N109" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O109" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P109" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q109" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="R109" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S109" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="T109" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="U109" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V109" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="W109" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="X109" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y109" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z109" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="110" spans="1:31">
       <c r="A110" t="s">
-        <v>172</v>
+        <v>291</v>
       </c>
       <c r="B110">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>56</v>
+        <v>267</v>
       </c>
       <c r="D110" t="s">
-        <v>173</v>
-      </c>
-      <c r="E110">
-        <v>719.14</v>
+        <v>292</v>
+      </c>
+      <c r="E110" t="s">
+        <v>812</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q110" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="R110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S110" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="T110" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="U110" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V110" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="W110" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="X110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y110" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z110" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="111" spans="1:31">
       <c r="A111" t="s">
-        <v>291</v>
+        <v>202</v>
       </c>
       <c r="B111">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="C111" t="s">
-        <v>267</v>
+        <v>27</v>
       </c>
       <c r="D111" t="s">
-        <v>292</v>
-      </c>
-      <c r="E111">
-        <v>2356.2</v>
+        <v>203</v>
+      </c>
+      <c r="E111" t="s">
+        <v>818</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L111" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q111" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="R111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S111" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="T111" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="U111" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V111" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="W111" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="X111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y111" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z111" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="112" spans="1:31">
       <c r="A112" t="s">
-        <v>202</v>
+        <v>70</v>
       </c>
       <c r="B112">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C112" t="s">
         <v>27</v>
       </c>
       <c r="D112" t="s">
-        <v>203</v>
-      </c>
-      <c r="E112">
-        <v>756.58</v>
+        <v>71</v>
+      </c>
+      <c r="E112" t="s">
+        <v>806</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q112" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="R112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S112" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="T112" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="U112" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V112" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="W112" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="X112" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="Y112" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z112" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="113" spans="1:31">
       <c r="A113" t="s">
-        <v>70</v>
+        <v>242</v>
       </c>
       <c r="B113">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C113" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="D113" t="s">
-        <v>71</v>
-      </c>
-      <c r="E113">
-        <v>719.14</v>
+        <v>243</v>
+      </c>
+      <c r="E113" t="s">
+        <v>826</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q113" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="R113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S113" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="T113" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="U113" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V113" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="W113" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="X113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y113" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z113" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="114" spans="1:31">
       <c r="A114" t="s">
-        <v>242</v>
+        <v>28</v>
       </c>
       <c r="B114">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C114" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="D114" t="s">
-        <v>243</v>
-      </c>
-      <c r="E114">
-        <v>3956.26</v>
+        <v>29</v>
+      </c>
+      <c r="E114" t="s">
+        <v>832</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L114" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="M114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q114" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="R114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S114" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="T114" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="U114" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V114" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="W114" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="X114" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="Y114" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z114" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="115" spans="1:31">
       <c r="A115" t="s">
-        <v>28</v>
+        <v>236</v>
       </c>
       <c r="B115">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="C115" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="D115" t="s">
-        <v>29</v>
-      </c>
-      <c r="E115">
-        <v>828.04</v>
+        <v>237</v>
+      </c>
+      <c r="E115" t="s">
+        <v>838</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="I115" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q115" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="R115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S115" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="T115" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="U115" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V115" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="W115" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y115" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z115" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="116" spans="1:31">
       <c r="A116" t="s">
-        <v>236</v>
+        <v>462</v>
       </c>
       <c r="B116">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="C116" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D116" t="s">
-        <v>237</v>
-      </c>
-      <c r="E116">
-        <v>757</v>
+        <v>463</v>
+      </c>
+      <c r="E116" t="s">
+        <v>843</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="I116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J116" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K116" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q116" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="R116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S116" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="T116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U116" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W116" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="X116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y116" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z116" s="1" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="117" spans="1:31">
       <c r="A117" t="s">
-        <v>462</v>
+        <v>255</v>
       </c>
       <c r="B117">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="C117" t="s">
-        <v>82</v>
+        <v>254</v>
       </c>
       <c r="D117" t="s">
-        <v>463</v>
-      </c>
-      <c r="E117">
-        <v>427.64</v>
+        <v>256</v>
+      </c>
+      <c r="E117" t="s">
+        <v>848</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="J117" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q117" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="R117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S117" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="T117" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="U117" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V117" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="W117" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="X117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y117" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z117" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="118" spans="1:31">
       <c r="A118" t="s">
-        <v>255</v>
+        <v>350</v>
       </c>
       <c r="B118">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="C118" t="s">
-        <v>254</v>
+        <v>82</v>
       </c>
       <c r="D118" t="s">
-        <v>256</v>
-      </c>
-      <c r="E118">
-        <v>1737.78</v>
+        <v>351</v>
+      </c>
+      <c r="E118" t="s">
+        <v>794</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="N118" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="O118" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="P118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q118" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S118" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="T118" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="U118" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="V118" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="W118" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y118" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z118" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="119" spans="1:31">
       <c r="A119" t="s">
-        <v>350</v>
+        <v>190</v>
       </c>
       <c r="B119">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C119" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="D119" t="s">
-        <v>351</v>
-      </c>
-      <c r="E119">
-        <v>543.06</v>
+        <v>191</v>
+      </c>
+      <c r="E119" t="s">
+        <v>857</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q119" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="R119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S119" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="T119" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="U119" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V119" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="W119" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y119" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z119" s="1" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="120" spans="1:31">
       <c r="A120" t="s">
-        <v>190</v>
+        <v>338</v>
       </c>
       <c r="B120">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="C120" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D120" t="s">
-        <v>191</v>
-      </c>
-      <c r="E120">
-        <v>394.94</v>
+        <v>339</v>
+      </c>
+      <c r="E120" t="s">
+        <v>369</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="J120" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L120" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q120" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="R120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S120" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="T120" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="U120" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V120" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="W120" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="X120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z120" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="121" spans="1:31">
       <c r="A121" t="s">
-        <v>338</v>
+        <v>416</v>
       </c>
       <c r="B121">
-        <v>39</v>
+        <v>80</v>
       </c>
       <c r="C121" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="D121" t="s">
-        <v>339</v>
-      </c>
-      <c r="E121">
-        <v>723.68</v>
+        <v>417</v>
+      </c>
+      <c r="E121" t="s">
+        <v>865</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="J121" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q121" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="R121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S121" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="T121" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="U121" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V121" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="W121" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="X121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y121" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z121" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="122" spans="1:31">
       <c r="A122" t="s">
-        <v>416</v>
+        <v>344</v>
       </c>
       <c r="B122">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C122" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="D122" t="s">
-        <v>417</v>
-      </c>
-      <c r="E122">
-        <v>642.28</v>
+        <v>345</v>
+      </c>
+      <c r="E122" t="s">
+        <v>794</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="J122" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q122" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="R122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S122" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="T122" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="U122" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V122" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="W122" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="X122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z122" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="123" spans="1:31">
       <c r="A123" t="s">
-        <v>344</v>
+        <v>160</v>
       </c>
       <c r="B123">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="C123" t="s">
-        <v>135</v>
+        <v>27</v>
       </c>
       <c r="D123" t="s">
-        <v>345</v>
-      </c>
-      <c r="E123">
-        <v>543.06</v>
+        <v>161</v>
+      </c>
+      <c r="E123" t="s">
+        <v>872</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="J123" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L123" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="M123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q123" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="R123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S123" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="T123" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="U123" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V123" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="W123" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="X123" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="Y123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z123" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="124" spans="1:31">
       <c r="A124" t="s">
-        <v>160</v>
+        <v>405</v>
       </c>
       <c r="B124">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="C124" t="s">
         <v>27</v>
       </c>
       <c r="D124" t="s">
-        <v>161</v>
-      </c>
-      <c r="E124">
-        <v>552.92</v>
+        <v>406</v>
+      </c>
+      <c r="E124" t="s">
+        <v>878</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="J124" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K124" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L124" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="M124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q124" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="R124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S124" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="T124" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="U124" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V124" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="W124" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z124" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="125" spans="1:31">
       <c r="A125" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="B125">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="C125" t="s">
         <v>27</v>
       </c>
       <c r="D125" t="s">
-        <v>406</v>
-      </c>
-      <c r="E125">
-        <v>690.8</v>
+        <v>389</v>
+      </c>
+      <c r="E125" t="s">
+        <v>883</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L125" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q125" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="R125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S125" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="T125" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="U125" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V125" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="W125" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z125" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="126" spans="1:31">
       <c r="A126" t="s">
-        <v>388</v>
+        <v>224</v>
       </c>
       <c r="B126">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="C126" t="s">
         <v>27</v>
       </c>
       <c r="D126" t="s">
-        <v>389</v>
-      </c>
-      <c r="E126">
-        <v>423.62</v>
+        <v>225</v>
+      </c>
+      <c r="E126" t="s">
+        <v>887</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q126" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="R126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S126" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="T126" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="U126" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V126" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="W126" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X126" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="Y126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z126" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="127" spans="1:31">
       <c r="A127" t="s">
-        <v>224</v>
+        <v>451</v>
       </c>
       <c r="B127">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="C127" t="s">
-        <v>27</v>
+        <v>267</v>
       </c>
       <c r="D127" t="s">
-        <v>225</v>
-      </c>
-      <c r="E127">
-        <v>506.84</v>
+        <v>452</v>
+      </c>
+      <c r="E127" t="s">
+        <v>893</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="J127" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q127" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="R127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S127" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="T127" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="U127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V127" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="W127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z127" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="128" spans="1:31">
       <c r="A128" t="s">
-        <v>451</v>
+        <v>122</v>
       </c>
       <c r="B128">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C128" t="s">
-        <v>267</v>
+        <v>56</v>
       </c>
       <c r="D128" t="s">
-        <v>452</v>
-      </c>
-      <c r="E128">
-        <v>1407.6</v>
+        <v>123</v>
+      </c>
+      <c r="E128" t="s">
+        <v>898</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q128" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="R128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S128" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="T128" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="U128" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V128" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="W128" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="X128" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="Y128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z128" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="129" spans="1:31">
       <c r="A129" t="s">
-        <v>122</v>
+        <v>434</v>
       </c>
       <c r="B129">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="C129" t="s">
-        <v>56</v>
+        <v>254</v>
       </c>
       <c r="D129" t="s">
-        <v>123</v>
-      </c>
-      <c r="E129">
-        <v>1135.48</v>
+        <v>435</v>
+      </c>
+      <c r="E129" t="s">
+        <v>787</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q129" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="R129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S129" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="T129" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="U129" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V129" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="W129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z129" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="130" spans="1:31">
       <c r="A130" t="s">
-        <v>434</v>
+        <v>355</v>
       </c>
       <c r="B130">
-        <v>103</v>
+        <v>12</v>
       </c>
       <c r="C130" t="s">
-        <v>254</v>
+        <v>82</v>
       </c>
       <c r="D130" t="s">
-        <v>435</v>
-      </c>
-      <c r="E130">
-        <v>657.9</v>
+        <v>356</v>
+      </c>
+      <c r="E130" t="s">
+        <v>906</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="J130" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K130" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q130" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="R130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S130" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="T130" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="U130" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V130" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="W130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X130" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="Y130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z130" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="131" spans="1:31">
       <c r="A131" t="s">
-        <v>355</v>
+        <v>472</v>
       </c>
       <c r="B131">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="C131" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="D131" t="s">
-        <v>356</v>
-      </c>
-      <c r="E131">
-        <v>828.4</v>
+        <v>473</v>
+      </c>
+      <c r="E131" t="s">
+        <v>912</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K131" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L131" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="M131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q131" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="R131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S131" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="T131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U131" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W131" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z131" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="132" spans="1:31">
       <c r="A132" t="s">
-        <v>472</v>
+        <v>280</v>
       </c>
       <c r="B132">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="C132" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="D132" t="s">
-        <v>473</v>
-      </c>
-      <c r="E132">
-        <v>592.1</v>
+        <v>281</v>
+      </c>
+      <c r="E132" t="s">
+        <v>916</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="J132" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K132" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q132" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="R132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S132" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="T132" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="U132" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V132" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="W132" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="X132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z132" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="133" spans="1:31">
       <c r="A133" t="s">
-        <v>280</v>
+        <v>399</v>
       </c>
       <c r="B133">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="C133" t="s">
         <v>82</v>
       </c>
       <c r="D133" t="s">
-        <v>281</v>
-      </c>
-      <c r="E133">
-        <v>2008.5</v>
+        <v>400</v>
+      </c>
+      <c r="E133" t="s">
+        <v>857</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I133" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="J133" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K133" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q133" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="R133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S133" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="T133" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="U133" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V133" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="W133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X133" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="Y133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z133" s="1" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="134" spans="1:31">
       <c r="A134" t="s">
-        <v>399</v>
+        <v>314</v>
       </c>
       <c r="B134">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C134" t="s">
         <v>82</v>
       </c>
       <c r="D134" t="s">
-        <v>400</v>
-      </c>
-      <c r="E134">
-        <v>394.94</v>
+        <v>315</v>
+      </c>
+      <c r="E134" t="s">
+        <v>124</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I134" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="J134" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K134" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q134" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="R134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S134" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="T134" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="U134" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V134" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="W134" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="X134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z134" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="135" spans="1:31">
       <c r="A135" t="s">
-        <v>314</v>
+        <v>109</v>
       </c>
       <c r="B135">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="C135" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="D135" t="s">
-        <v>315</v>
-      </c>
-      <c r="E135">
-        <v>567.74</v>
+        <v>110</v>
+      </c>
+      <c r="E135" t="s">
+        <v>838</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="I135" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="J135" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K135" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q135" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="R135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S135" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="T135" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="U135" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V135" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="W135" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="X135" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="Y135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z135" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="136" spans="1:31">
       <c r="A136" t="s">
-        <v>109</v>
+        <v>326</v>
       </c>
       <c r="B136">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="C136" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="D136" t="s">
-        <v>110</v>
-      </c>
-      <c r="E136">
-        <v>757</v>
+        <v>327</v>
+      </c>
+      <c r="E136" t="s">
+        <v>928</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="I136" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="J136" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K136" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q136" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="R136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S136" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="T136" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="U136" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V136" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="W136" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="X136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z136" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="137" spans="1:31">
       <c r="A137" t="s">
-        <v>326</v>
+        <v>367</v>
       </c>
       <c r="B137">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="C137" t="s">
-        <v>82</v>
+        <v>267</v>
       </c>
       <c r="D137" t="s">
-        <v>327</v>
-      </c>
-      <c r="E137">
-        <v>2877.8</v>
+        <v>368</v>
+      </c>
+      <c r="E137" t="s">
+        <v>934</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H137" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="I137" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="J137" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q137" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="R137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S137" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="T137" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="U137" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V137" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="W137" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="X137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z137" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="138" spans="1:31">
       <c r="A138" t="s">
-        <v>367</v>
+        <v>136</v>
       </c>
       <c r="B138">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="C138" t="s">
-        <v>267</v>
+        <v>135</v>
       </c>
       <c r="D138" t="s">
-        <v>368</v>
-      </c>
-      <c r="E138">
-        <v>1447.36</v>
+        <v>137</v>
+      </c>
+      <c r="E138" t="s">
+        <v>940</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="I138" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L138" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q138" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="R138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S138" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="T138" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="U138" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V138" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="W138" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X138" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="Y138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z138" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="139" spans="1:31">
       <c r="A139" t="s">
-        <v>136</v>
+        <v>268</v>
       </c>
       <c r="B139">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="C139" t="s">
-        <v>135</v>
+        <v>267</v>
       </c>
       <c r="D139" t="s">
-        <v>137</v>
-      </c>
-      <c r="E139">
-        <v>687.88</v>
+        <v>269</v>
+      </c>
+      <c r="E139" t="s">
+        <v>946</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="I139" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="J139" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K139" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P139" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q139" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="R139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S139" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="T139" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="U139" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V139" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="W139" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="X139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z139" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="140" spans="1:31">
       <c r="A140" t="s">
-        <v>268</v>
+        <v>428</v>
       </c>
       <c r="B140">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="C140" t="s">
         <v>267</v>
       </c>
       <c r="D140" t="s">
-        <v>269</v>
-      </c>
-      <c r="E140">
-        <v>4111.84</v>
+        <v>429</v>
+      </c>
+      <c r="E140" t="s">
+        <v>951</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H140" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="I140" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="J140" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K140" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q140" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="R140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S140" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="T140" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="U140" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V140" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="W140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z140" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="141" spans="1:31">
       <c r="A141" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="B141">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C141" t="s">
         <v>267</v>
       </c>
       <c r="D141" t="s">
-        <v>429</v>
-      </c>
-      <c r="E141">
-        <v>1448.16</v>
+        <v>441</v>
+      </c>
+      <c r="E141" t="s">
+        <v>956</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H141" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="I141" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="J141" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q141" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="R141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S141" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="T141" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="U141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V141" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="W141" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="X141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z141" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="142" spans="1:31">
       <c r="A142" t="s">
-        <v>440</v>
+        <v>303</v>
       </c>
       <c r="B142">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="C142" t="s">
-        <v>267</v>
+        <v>82</v>
       </c>
       <c r="D142" t="s">
-        <v>441</v>
-      </c>
-      <c r="E142">
-        <v>4310.82</v>
+        <v>304</v>
+      </c>
+      <c r="E142" t="s">
+        <v>369</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H142" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="I142" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="J142" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K142" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q142" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="R142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S142" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="T142" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="U142" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V142" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="W142" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z142" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="143" spans="1:31">
       <c r="A143" t="s">
-        <v>303</v>
+        <v>96</v>
       </c>
       <c r="B143">
-        <v>79</v>
+        <v>26</v>
       </c>
       <c r="C143" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D143" t="s">
-        <v>304</v>
-      </c>
-      <c r="E143">
-        <v>723.68</v>
-      </c>
-    </row>
-    <row r="144" spans="1:31">
-      <c r="A144" t="s">
-        <v>96</v>
-      </c>
-      <c r="B144">
-        <v>26</v>
-      </c>
-      <c r="C144" t="s">
-        <v>95</v>
-      </c>
-      <c r="D144" t="s">
         <v>97</v>
       </c>
-      <c r="E144">
-        <v>1448.16</v>
+      <c r="E143" t="s">
+        <v>951</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H143" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="J143" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="K143" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="L143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q143" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="R143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S143" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="T143" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="U143" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="V143" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="W143" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="X143" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="Y143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z143" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>